<commit_message>
Seeder de las bases de datos
</commit_message>
<xml_diff>
--- a/datos/productos.xlsx
+++ b/datos/productos.xlsx
@@ -17,17 +17,17 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">productos!$A$1:$I$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">servicios!$A$1:$C$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">servicios!$A$1:$F$77</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabla1[#All]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">productos!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">servicios!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="269">
   <si>
     <t>folio</t>
   </si>
@@ -560,9 +560,6 @@
     <t>Biopsia 4 cm</t>
   </si>
   <si>
-    <t>Copìas/Platino</t>
-  </si>
-  <si>
     <t>Quimica Sanguinea 12</t>
   </si>
   <si>
@@ -729,6 +726,114 @@
   </si>
   <si>
     <t>Vendas</t>
+  </si>
+  <si>
+    <t>largo</t>
+  </si>
+  <si>
+    <t>nomb_corto</t>
+  </si>
+  <si>
+    <t>nom_corto largo</t>
+  </si>
+  <si>
+    <t>Anal.Leucosis Bovina</t>
+  </si>
+  <si>
+    <t>Anal.LenguaAzul</t>
+  </si>
+  <si>
+    <t>Anal.BrucellasOvis</t>
+  </si>
+  <si>
+    <t>Anemia Inf. Equina</t>
+  </si>
+  <si>
+    <t>Brucella (T.Chis)</t>
+  </si>
+  <si>
+    <t>Busq. Hemoparasitos</t>
+  </si>
+  <si>
+    <t>Cult. Antibiogramas</t>
+  </si>
+  <si>
+    <t>Cast. Gat. Hemb.</t>
+  </si>
+  <si>
+    <t>Cast. Gat. Mach.</t>
+  </si>
+  <si>
+    <t>Cast. Perros</t>
+  </si>
+  <si>
+    <t>Cir. Gra. Orejas</t>
+  </si>
+  <si>
+    <t>Cir. Mnr. Orejas</t>
+  </si>
+  <si>
+    <t>Copro Bov./Equ.</t>
+  </si>
+  <si>
+    <t>Copro Fel/Can</t>
+  </si>
+  <si>
+    <t>Cultivo.Bact.</t>
+  </si>
+  <si>
+    <t>Cult. LecheyAntibi.</t>
+  </si>
+  <si>
+    <t>Envio.Paque.</t>
+  </si>
+  <si>
+    <t>Ester.Perro Ch</t>
+  </si>
+  <si>
+    <t>Ester.Perro Gde</t>
+  </si>
+  <si>
+    <t>Estrt. Gatos</t>
+  </si>
+  <si>
+    <t>Fij. Complemento</t>
+  </si>
+  <si>
+    <t>Limp. Detal P. Ch</t>
+  </si>
+  <si>
+    <t>Piroplasmosis Equina</t>
+  </si>
+  <si>
+    <t>Rasp. (acar/hong)</t>
+  </si>
+  <si>
+    <t>Rec. Cels Somaticas</t>
+  </si>
+  <si>
+    <t>Acido Urico</t>
+  </si>
+  <si>
+    <t>Anal. Durina</t>
+  </si>
+  <si>
+    <t>Anal. Muermo</t>
+  </si>
+  <si>
+    <t>Bilirrubinal Total</t>
+  </si>
+  <si>
+    <t>Biometrica Hematica</t>
+  </si>
+  <si>
+    <t>Carat.Dict</t>
+  </si>
+  <si>
+    <t>Copias/Platino</t>
+  </si>
+  <si>
+    <t>AnalitiHorm4Horonas</t>
   </si>
 </sst>
 </file>
@@ -909,7 +1014,137 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -975,6 +1210,114 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -998,6 +1341,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1005,15 +1357,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1049,194 +1392,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1251,30 +1406,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:I88" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:I88" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:I88"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="folio" dataDxfId="19"/>
-    <tableColumn id="2" name="nombre" dataDxfId="18"/>
-    <tableColumn id="3" name="precio_venta" dataDxfId="17"/>
-    <tableColumn id="4" name="serie_ini" dataDxfId="16"/>
-    <tableColumn id="5" name="serie_fini" dataDxfId="15"/>
-    <tableColumn id="6" name="cantidad" dataDxfId="14"/>
-    <tableColumn id="7" name="presentacion" dataDxfId="13"/>
-    <tableColumn id="8" name="linea" dataDxfId="12"/>
-    <tableColumn id="9" name="marca" dataDxfId="11"/>
+    <tableColumn id="1" name="folio" dataDxfId="18"/>
+    <tableColumn id="2" name="nombre" dataDxfId="17"/>
+    <tableColumn id="3" name="precio_venta" dataDxfId="16"/>
+    <tableColumn id="4" name="serie_ini" dataDxfId="15"/>
+    <tableColumn id="5" name="serie_fini" dataDxfId="14"/>
+    <tableColumn id="6" name="cantidad" dataDxfId="13"/>
+    <tableColumn id="7" name="presentacion" dataDxfId="12"/>
+    <tableColumn id="8" name="linea" dataDxfId="11"/>
+    <tableColumn id="9" name="marca" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C77" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C77"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="folio" dataDxfId="3"/>
-    <tableColumn id="2" name="nombre" dataDxfId="2"/>
-    <tableColumn id="3" name="precio_venta" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F77" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F77"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="folio" dataDxfId="5"/>
+    <tableColumn id="2" name="nombre" dataDxfId="4"/>
+    <tableColumn id="4" name="largo" dataDxfId="2">
+      <calculatedColumnFormula>LEN(Tabla2[[#This Row],[nombre]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="nomb_corto" dataDxfId="1"/>
+    <tableColumn id="6" name="nom_corto largo" dataDxfId="0">
+      <calculatedColumnFormula>LEN(Tabla2[[#This Row],[nomb_corto]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="precio_venta" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1546,7 +1708,7 @@
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1594,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1609,13 +1771,13 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1623,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -1638,13 +1800,13 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1927,7 +2089,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1950,7 +2112,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1973,7 +2135,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1996,7 +2158,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -2019,7 +2181,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -2042,7 +2204,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -2175,7 +2337,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
@@ -2198,7 +2360,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C26" s="1">
         <v>250</v>
@@ -2319,7 +2481,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -2460,7 +2622,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C36" s="1">
         <v>130</v>
@@ -2483,7 +2645,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37" s="1">
         <v>150</v>
@@ -2506,7 +2668,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C38" s="1">
         <v>100</v>
@@ -2529,7 +2691,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C39" s="1">
         <v>280</v>
@@ -2545,7 +2707,7 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>140</v>
@@ -2782,7 +2944,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C48" s="1">
         <v>130</v>
@@ -2805,7 +2967,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C49" s="1">
         <v>100</v>
@@ -2959,7 +3121,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
@@ -3009,7 +3171,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C57" s="1">
         <v>200</v>
@@ -3163,7 +3325,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C63" s="1">
         <v>60</v>
@@ -3244,7 +3406,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C66" s="1">
         <v>0</v>
@@ -3319,7 +3481,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C69" s="1">
         <v>3</v>
@@ -3342,7 +3504,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C70" s="1">
         <v>10</v>
@@ -3394,7 +3556,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C72" s="1">
         <v>0</v>
@@ -3411,7 +3573,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3419,7 +3581,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C73" s="1">
         <v>0</v>
@@ -3626,7 +3788,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C82" s="1">
         <v>150</v>
@@ -3676,7 +3838,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
@@ -3786,7 +3948,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C88" s="5">
         <v>300</v>
@@ -3801,11 +3963,11 @@
         <v>1</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3826,19 +3988,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3846,10 +4011,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>18</v>
       </c>
@@ -3857,32 +4031,77 @@
         <v>26</v>
       </c>
       <c r="C2" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>11</v>
+      </c>
+      <c r="F2" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="H2" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Acido urico', 'nomb_corto'=&gt; 'Acido Urico','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>8</v>
+      </c>
+      <c r="F3" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="H3" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Albumina', 'nomb_corto'=&gt; 'Albumina','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="H4" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'ALT TG', 'nomb_corto'=&gt; 'ALT TG','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>27</v>
       </c>
@@ -3890,10 +4109,25 @@
         <v>35</v>
       </c>
       <c r="C5" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="H5" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analisis de brucella Ovis', 'nomb_corto'=&gt; 'Anal.BrucellasOvis','precio'=&gt; 80]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>21</v>
       </c>
@@ -3901,10 +4135,25 @@
         <v>29</v>
       </c>
       <c r="C6" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="H6" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analisis de durina', 'nomb_corto'=&gt; 'Anal. Durina','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>25</v>
       </c>
@@ -3912,10 +4161,25 @@
         <v>33</v>
       </c>
       <c r="C7" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F7" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="H7" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analisis de lengua azul', 'nomb_corto'=&gt; 'Anal.LenguaAzul','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>24</v>
       </c>
@@ -3923,10 +4187,25 @@
         <v>32</v>
       </c>
       <c r="C8" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>20</v>
+      </c>
+      <c r="F8" s="3">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="H8" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analisis de leucosis bovina', 'nomb_corto'=&gt; 'Anal.Leucosis Bovina','precio'=&gt; 250]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>22</v>
       </c>
@@ -3934,10 +4213,25 @@
         <v>30</v>
       </c>
       <c r="C9" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F9" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="H9" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analisis de muermo', 'nomb_corto'=&gt; 'Anal. Muermo','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>51</v>
       </c>
@@ -3945,10 +4239,25 @@
         <v>170</v>
       </c>
       <c r="C10" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F10" s="3">
         <v>550</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="H10" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Analitica hormonal 4 horonas', 'nomb_corto'=&gt; 'AnalitiHorm4Horonas','precio'=&gt; 550]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>40</v>
       </c>
@@ -3956,32 +4265,77 @@
         <v>65</v>
       </c>
       <c r="C11" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F11" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="H11" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Anemia Infecciosa Equina', 'nomb_corto'=&gt; 'Anemia Inf. Equina','precio'=&gt; 500]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="H12" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'AST TG', 'nomb_corto'=&gt; 'AST TG','precio'=&gt; 80]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F13" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="H13" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Bilirrubina total', 'nomb_corto'=&gt; 'Bilirrubinal Total','precio'=&gt; 80]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>32</v>
       </c>
@@ -3989,10 +4343,25 @@
         <v>53</v>
       </c>
       <c r="C14" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F14" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="H14" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Biometria Hematica', 'nomb_corto'=&gt; 'Biometrica Hematica','precio'=&gt; 150]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>55</v>
       </c>
@@ -4000,10 +4369,25 @@
         <v>176</v>
       </c>
       <c r="C15" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>12</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F15" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="H15" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Biopsia 4 cm', 'nomb_corto'=&gt; 'Biopsia 4 cm','precio'=&gt; 1000]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>54</v>
       </c>
@@ -4011,10 +4395,25 @@
         <v>175</v>
       </c>
       <c r="C16" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F16" s="3">
         <v>1400</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="H16" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Biopsia 7 cm', 'nomb_corto'=&gt; 'Biopsia 7 cm','precio'=&gt; 1400]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>30</v>
       </c>
@@ -4022,10 +4421,25 @@
         <v>43</v>
       </c>
       <c r="C17" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E17" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="H17" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Brucella (Tarjeta-CHIS)', 'nomb_corto'=&gt; 'Brucella (T.Chis)','precio'=&gt; 5]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>38</v>
       </c>
@@ -4033,10 +4447,25 @@
         <v>63</v>
       </c>
       <c r="C18" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>9</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>9</v>
+      </c>
+      <c r="F18" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="H18" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Brucellas', 'nomb_corto'=&gt; 'Brucellas','precio'=&gt; 7]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -4044,10 +4473,25 @@
         <v>10</v>
       </c>
       <c r="C19" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>26</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E19" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F19" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="H19" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Busquedas de Hemoparasitos', 'nomb_corto'=&gt; 'Busq. Hemoparasitos','precio'=&gt; 100]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -4055,10 +4499,25 @@
         <v>20</v>
       </c>
       <c r="C20" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>6</v>
+      </c>
+      <c r="F20" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="H20" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Calcio', 'nomb_corto'=&gt; 'Calcio','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>44</v>
       </c>
@@ -4066,43 +4525,103 @@
         <v>72</v>
       </c>
       <c r="C21" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E21" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>10</v>
+      </c>
+      <c r="F21" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="H21" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Caratula Dictamen', 'nomb_corto'=&gt; 'Carat.Dict','precio'=&gt; 30]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C22" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E22" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F22" s="3">
         <v>850</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="H22" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Castraccion gatos hembras', 'nomb_corto'=&gt; 'Cast. Gat. Hemb.','precio'=&gt; 850]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C23" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F23" s="3">
         <v>700</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="H23" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Castraccion gatos machos', 'nomb_corto'=&gt; 'Cast. Gat. Mach.','precio'=&gt; 700]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F24" s="3">
         <v>1500</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="H24" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Castraccion perros 1500', 'nomb_corto'=&gt; 'Cast. Perros','precio'=&gt; 1500]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>33</v>
       </c>
@@ -4110,10 +4629,25 @@
         <v>55</v>
       </c>
       <c r="C25" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F25" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="H25" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Check-Up 4DX', 'nomb_corto'=&gt; 'Check-Up 4DX','precio'=&gt; 500]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>35</v>
       </c>
@@ -4121,10 +4655,25 @@
         <v>57</v>
       </c>
       <c r="C26" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>17</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F26" s="3">
         <v>1400</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="H26" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Check-up Completo', 'nomb_corto'=&gt; 'Check-up Completo','precio'=&gt; 1400]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>34</v>
       </c>
@@ -4132,10 +4681,25 @@
         <v>56</v>
       </c>
       <c r="C27" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>11</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>11</v>
+      </c>
+      <c r="F27" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="H27" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Chek-up +Bh', 'nomb_corto'=&gt; 'Chek-up +Bh','precio'=&gt; 600]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
         <v>49</v>
       </c>
@@ -4143,10 +4707,25 @@
         <v>148</v>
       </c>
       <c r="C28" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E28" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F28" s="3">
         <v>1800</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="H28" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Cirugias Gra. Orejas', 'nomb_corto'=&gt; 'Cir. Gra. Orejas','precio'=&gt; 1800]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
         <v>50</v>
       </c>
@@ -4154,10 +4733,25 @@
         <v>158</v>
       </c>
       <c r="C29" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E29" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F29" s="3">
         <v>1500</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="H29" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Cirugias menor Oreja', 'nomb_corto'=&gt; 'Cir. Mnr. Orejas','precio'=&gt; 1500]</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
         <v>19</v>
       </c>
@@ -4165,10 +4759,25 @@
         <v>27</v>
       </c>
       <c r="C30" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>10</v>
+      </c>
+      <c r="F30" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="H30" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Colesterol', 'nomb_corto'=&gt; 'Colesterol','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
         <v>45</v>
       </c>
@@ -4176,10 +4785,25 @@
         <v>73</v>
       </c>
       <c r="C31" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F31" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="H31" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Complementarias', 'nomb_corto'=&gt; 'Complementarias','precio'=&gt; 25]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>36</v>
       </c>
@@ -4187,21 +4811,51 @@
         <v>58</v>
       </c>
       <c r="C32" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>9</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>9</v>
+      </c>
+      <c r="F32" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="H32" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Consultas', 'nomb_corto'=&gt; 'Consultas','precio'=&gt; 200]</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="C33" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E33" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>14</v>
+      </c>
+      <c r="F33" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="H33" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Copias/Platino', 'nomb_corto'=&gt; 'Copias/Platino','precio'=&gt; 1]</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -4209,10 +4863,25 @@
         <v>9</v>
       </c>
       <c r="C34" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>21</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E34" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F34" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="H34" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Copro Bovinos/Equinos', 'nomb_corto'=&gt; 'Copro Bov./Equ.','precio'=&gt; 60]</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>28</v>
       </c>
@@ -4220,10 +4889,25 @@
         <v>36</v>
       </c>
       <c r="C35" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E35" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>13</v>
+      </c>
+      <c r="F35" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="H35" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Copro felinos y Caninos', 'nomb_corto'=&gt; 'Copro Fel/Can','precio'=&gt; 100]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
         <v>31</v>
       </c>
@@ -4231,21 +4915,51 @@
         <v>52</v>
       </c>
       <c r="C36" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>11</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>11</v>
+      </c>
+      <c r="F36" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="H36" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Copro Ovino', 'nomb_corto'=&gt; 'Copro Ovino','precio'=&gt; 60]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
         <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F37" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="H37" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Creatinfosfokinasa', 'nomb_corto'=&gt; 'Creatinfosfokinasa','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
         <v>17</v>
       </c>
@@ -4253,21 +4967,51 @@
         <v>25</v>
       </c>
       <c r="C38" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>10</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>10</v>
+      </c>
+      <c r="F38" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="H38" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Creatinina', 'nomb_corto'=&gt; 'Creatinina','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="2">
         <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C39" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>22</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E39" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>13</v>
+      </c>
+      <c r="F39" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="H39" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Cultivo bacteriologico', 'nomb_corto'=&gt; 'Cultivo.Bact.','precio'=&gt; 500]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="2">
         <v>9</v>
       </c>
@@ -4275,10 +5019,25 @@
         <v>17</v>
       </c>
       <c r="C40" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>32</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E40" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F40" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="H40" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Cultivos de leche y antibiograma', 'nomb_corto'=&gt; 'Cult. LecheyAntibi.','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="2">
         <v>26</v>
       </c>
@@ -4286,10 +5045,25 @@
         <v>34</v>
       </c>
       <c r="C41" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>24</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E41" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F41" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="H41" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Cultivos y Antibiogramas', 'nomb_corto'=&gt; 'Cult. Antibiogramas','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
         <v>47</v>
       </c>
@@ -4297,10 +5071,25 @@
         <v>75</v>
       </c>
       <c r="C42" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F42" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="H42" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Curacion general', 'nomb_corto'=&gt; 'Curacion general','precio'=&gt; 200]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="2">
         <v>46</v>
       </c>
@@ -4308,10 +5097,25 @@
         <v>74</v>
       </c>
       <c r="C43" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>13</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>13</v>
+      </c>
+      <c r="F43" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="H43" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Dict. Externo', 'nomb_corto'=&gt; 'Dict. Externo','precio'=&gt; 35]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -4319,10 +5123,25 @@
         <v>70</v>
       </c>
       <c r="C44" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>11</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>11</v>
+      </c>
+      <c r="F44" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="H44" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Envio Teapa', 'nomb_corto'=&gt; 'Envio Teapa','precio'=&gt; 49]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="2">
         <v>41</v>
       </c>
@@ -4330,10 +5149,25 @@
         <v>66</v>
       </c>
       <c r="C45" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E45" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F45" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="H45" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Envios de Paqueteria', 'nomb_corto'=&gt; 'Envio.Paque.','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>53</v>
       </c>
@@ -4341,43 +5175,103 @@
         <v>174</v>
       </c>
       <c r="C46" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F46" s="3">
         <v>400</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="H46" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Espermatobioscopia', 'nomb_corto'=&gt; 'Espermatobioscopia','precio'=&gt; 400]</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="2">
         <v>75</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>26</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E47" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>14</v>
+      </c>
+      <c r="F47" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="H47" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Esteriliazcion perro chico', 'nomb_corto'=&gt; 'Ester.Perro Ch','precio'=&gt; 2000]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="2">
         <v>76</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C48" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>27</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E48" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F48" s="3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="H48" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Esteriliazcion perro grande', 'nomb_corto'=&gt; 'Ester.Perro Gde','precio'=&gt; 2500]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="2">
         <v>68</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C49" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E49" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F49" s="3">
         <v>1200</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="H49" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Esterilizacion gatos', 'nomb_corto'=&gt; 'Estrt. Gatos','precio'=&gt; 1200]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="2">
         <v>6</v>
       </c>
@@ -4385,10 +5279,25 @@
         <v>14</v>
       </c>
       <c r="C50" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F50" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="H50" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Examen de Orina', 'nomb_corto'=&gt; 'Examen de Orina','precio'=&gt; 100]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="2">
         <v>39</v>
       </c>
@@ -4396,10 +5305,25 @@
         <v>64</v>
       </c>
       <c r="C51" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F51" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="H51" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Exudado Vaginal', 'nomb_corto'=&gt; 'Exudado Vaginal','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="2">
         <v>37</v>
       </c>
@@ -4407,10 +5331,25 @@
         <v>59</v>
       </c>
       <c r="C52" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E52" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F52" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="H52" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Fijacion de Complemento', 'nomb_corto'=&gt; 'Fij. Complemento','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="2">
         <v>13</v>
       </c>
@@ -4418,21 +5357,51 @@
         <v>21</v>
       </c>
       <c r="C53" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>7</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>7</v>
+      </c>
+      <c r="F53" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="H53" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Fosforo', 'nomb_corto'=&gt; 'Fosforo','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="2">
         <v>63</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C54" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>9</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>9</v>
+      </c>
+      <c r="F54" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="H54" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Globulina', 'nomb_corto'=&gt; 'Globulina','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="2">
         <v>15</v>
       </c>
@@ -4440,21 +5409,51 @@
         <v>23</v>
       </c>
       <c r="C55" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>7</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>7</v>
+      </c>
+      <c r="F55" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="H55" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Glucosa', 'nomb_corto'=&gt; 'Glucosa','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="2">
         <v>70</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C56" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>12</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F56" s="3">
         <v>365</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="H56" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Hipoteroides', 'nomb_corto'=&gt; 'Hipoteroides','precio'=&gt; 365]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="2">
         <v>48</v>
       </c>
@@ -4462,10 +5461,25 @@
         <v>145</v>
       </c>
       <c r="C57" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>17</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E57" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F57" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="H57" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Inyeccion general', 'nomb_corto'=&gt; 'Inyeccion general','precio'=&gt; 50]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="2">
         <v>29</v>
       </c>
@@ -4473,10 +5487,25 @@
         <v>37</v>
       </c>
       <c r="C58" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>10</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>10</v>
+      </c>
+      <c r="F58" s="3">
         <v>90</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="H58" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Leptospira', 'nomb_corto'=&gt; 'Leptospira','precio'=&gt; 90]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="2">
         <v>42</v>
       </c>
@@ -4484,32 +5513,77 @@
         <v>68</v>
       </c>
       <c r="C59" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>23</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E59" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F59" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="H59" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Limpieza Dental P.Chico', 'nomb_corto'=&gt; 'Limp. Detal P. Ch','precio'=&gt; 600]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="2">
         <v>62</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C60" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>16</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>16</v>
+      </c>
+      <c r="F60" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="H60" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Nitrogeno ureico', 'nomb_corto'=&gt; 'Nitrogeno ureico','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="2">
         <v>71</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E61" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>10</v>
+      </c>
+      <c r="F61" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="H61" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Parvovirus', 'nomb_corto'=&gt; 'Parvovirus','precio'=&gt; 500]</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="2">
         <v>7</v>
       </c>
@@ -4517,10 +5591,25 @@
         <v>15</v>
       </c>
       <c r="C62" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F62" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="H62" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Perfil Cardiaco', 'nomb_corto'=&gt; 'Perfil Cardiaco','precio'=&gt; 300]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="2">
         <v>4</v>
       </c>
@@ -4528,10 +5617,25 @@
         <v>12</v>
       </c>
       <c r="C63" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F63" s="3">
         <v>240</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="H63" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Perfil Hepatico', 'nomb_corto'=&gt; 'Perfil Hepatico','precio'=&gt; 240]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="2">
         <v>52</v>
       </c>
@@ -4539,10 +5643,25 @@
         <v>171</v>
       </c>
       <c r="C64" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>18</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E64" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>18</v>
+      </c>
+      <c r="F64" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="H64" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Perfil pancreatico', 'nomb_corto'=&gt; 'Perfil pancreatico','precio'=&gt; 200]</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="2">
         <v>5</v>
       </c>
@@ -4550,10 +5669,25 @@
         <v>13</v>
       </c>
       <c r="C65" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>12</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>12</v>
+      </c>
+      <c r="F65" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="H65" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Perfil Renal', 'nomb_corto'=&gt; 'Perfil Renal','precio'=&gt; 300]</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="2">
         <v>23</v>
       </c>
@@ -4561,43 +5695,103 @@
         <v>31</v>
       </c>
       <c r="C66" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E66" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>20</v>
+      </c>
+      <c r="F66" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="H66" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Piroplasmosis equina', 'nomb_corto'=&gt; 'Piroplasmosis Equina','precio'=&gt; 350]</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="2">
         <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C67" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>17</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E67" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F67" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="H67" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Proteinas totales', 'nomb_corto'=&gt; 'Proteinas totales','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="2">
         <v>59</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C68" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>15</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E68" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>15</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="H68" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Quimica Clinica', 'nomb_corto'=&gt; 'Quimica Clinica','precio'=&gt; 0]</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="2">
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C69" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>20</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E69" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>20</v>
+      </c>
+      <c r="F69" s="3">
         <v>800</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="H69" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Quimica Sanguinea 12', 'nomb_corto'=&gt; 'Quimica Sanguinea 12','precio'=&gt; 800]</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="2">
         <v>8</v>
       </c>
@@ -4605,21 +5799,51 @@
         <v>16</v>
       </c>
       <c r="C70" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>19</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F70" s="3">
         <v>240</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="H70" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Quimica Sanguinea 4', 'nomb_corto'=&gt; 'Quimica Sanguinea 4','precio'=&gt; 240]</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="2">
         <v>58</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>19</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E71" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F71" s="3">
         <v>400</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="H71" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Quimica Sanguinea 6', 'nomb_corto'=&gt; 'Quimica Sanguinea 6','precio'=&gt; 400]</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="2">
         <v>3</v>
       </c>
@@ -4627,10 +5851,25 @@
         <v>11</v>
       </c>
       <c r="C72" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>25</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E72" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>17</v>
+      </c>
+      <c r="F72" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="H72" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Raspado (acaros y hongos)', 'nomb_corto'=&gt; 'Rasp. (acar/hong)','precio'=&gt; 150]</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="2">
         <v>14</v>
       </c>
@@ -4638,10 +5877,25 @@
         <v>22</v>
       </c>
       <c r="C73" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>30</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E73" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>19</v>
+      </c>
+      <c r="F73" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="H73" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Recuentos de celulas somaticas', 'nomb_corto'=&gt; 'Rec. Cels Somaticas','precio'=&gt; 150]</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="2">
         <v>10</v>
       </c>
@@ -4649,10 +5903,25 @@
         <v>18</v>
       </c>
       <c r="C74" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>2</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>2</v>
+      </c>
+      <c r="F74" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="H74" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'TP', 'nomb_corto'=&gt; 'TP','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="2">
         <v>11</v>
       </c>
@@ -4660,10 +5929,25 @@
         <v>19</v>
       </c>
       <c r="C75" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>3</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>3</v>
+      </c>
+      <c r="F75" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="H75" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'TPT', 'nomb_corto'=&gt; 'TPT','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="2">
         <v>20</v>
       </c>
@@ -4671,10 +5955,25 @@
         <v>28</v>
       </c>
       <c r="C76" s="3">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>13</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="3">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>13</v>
+      </c>
+      <c r="F76" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="H76" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Trigliceridos', 'nomb_corto'=&gt; 'Trigliceridos','precio'=&gt; 70]</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="4">
         <v>16</v>
       </c>
@@ -4682,7 +5981,22 @@
         <v>24</v>
       </c>
       <c r="C77" s="6">
+        <f>LEN(Tabla2[[#This Row],[nombre]])</f>
+        <v>4</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="6">
+        <f>LEN(Tabla2[[#This Row],[nomb_corto]])</f>
+        <v>4</v>
+      </c>
+      <c r="F77" s="6">
         <v>70</v>
+      </c>
+      <c r="H77" t="str">
+        <f>"['nombre'=&gt; '"&amp;Tabla2[[#This Row],[nombre]]&amp;"', 'nomb_corto'=&gt; '"&amp;Tabla2[[#This Row],[nomb_corto]]&amp;"','precio'=&gt; "&amp;Tabla2[[#This Row],[precio_venta]]&amp;"]"</f>
+        <v>['nombre'=&gt; 'Urea', 'nomb_corto'=&gt; 'Urea','precio'=&gt; 70]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>